<commit_message>
Correction des prochains adversaires
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_04_07.xlsx
+++ b/Excel/TI/Mon_TI_2024_04_07.xlsx
@@ -2582,11 +2582,7 @@
           <t>Deni Avdija</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Questionable</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
           <t>F</t>

</xml_diff>